<commit_message>
Minor changes to results and documentation of config file
</commit_message>
<xml_diff>
--- a/Results_and_analysis/Dependence_tensor_on_fisher_kappa_analysis/results_analysis_complete_fisher_kappa.xlsx
+++ b/Results_and_analysis/Dependence_tensor_on_fisher_kappa_analysis/results_analysis_complete_fisher_kappa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plocha\Bachelor_thesis\Results_and_analysis\Dependence_tensor_on_fisher_kappa_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plocha\Bachelor_thesis\Python_scripts\Results_and_analysis\Dependence_tensor_on_fisher_kappa_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2D8E5-1B30-4F2C-94BD-960FFC92A94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A73BF6-3A5F-44E6-9776-1A22D2FBD633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5660,7 +5660,7 @@
   <dimension ref="A1:X2186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AB34" sqref="AB34"/>
+      <selection activeCell="Y65" sqref="Y65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>